<commit_message>
working on isolating leaf from background
</commit_message>
<xml_diff>
--- a/hair_model_results.xlsx
+++ b/hair_model_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,126 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>004-PI588478_15-3</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.9857791880580289</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>001-PI588568_13-107</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.8493184792593224</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>009-PI588470_15-17</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.9720587635652564</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>012-PI588471_15-23</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.7082437918797061</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>007-PI588601_15-11</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.6993877289623024</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>006-PI588606_15-9</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.9926110729154066</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>011-PI588463_15-21</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8298248193246827</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>010-PI588543_15-19</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.9614144369530073</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>002-PI588331_13-109</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.9649735094556326</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>003-PI597269_15-1</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.8681984001287604</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>008-PI588487_15-15</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.8292395127984116</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>005-PI588133_15-5</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.9903248612495549</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>